<commit_message>
hurda tesviki ve faiz indirimi
</commit_message>
<xml_diff>
--- a/r_input/hurda_tesviki.xlsx
+++ b/r_input/hurda_tesviki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72730B54-FFF5-4BDF-9798-53A7EB1A7C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA9814A-C44C-4107-9C2D-D724700E90E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A28CCFF-135B-4345-98CD-4416B433170E}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -96,7 +96,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>3000000000</v>
+        <v>2000000000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deneme yanilma 1.5 milyon hedef
</commit_message>
<xml_diff>
--- a/r_input/hurda_tesviki.xlsx
+++ b/r_input/hurda_tesviki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1828C25B-EFAC-40D4-B3EE-16220DE29480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFABFB62-2567-4CA8-BCFD-76A1364FFBC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5A28CCFF-135B-4345-98CD-4416B433170E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A28CCFF-135B-4345-98CD-4416B433170E}"/>
   </bookViews>
   <sheets>
     <sheet name="binek_arac" sheetId="1" r:id="rId1"/>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CCE55F-1B0A-4E57-81A5-BBA6925D903A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A069E5F-A95C-4EFD-A754-6B82568E03B6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
KPMG degisiklikleri ve otv_yakit grubu özet tablosu
</commit_message>
<xml_diff>
--- a/r_input/hurda_tesviki.xlsx
+++ b/r_input/hurda_tesviki.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcinar\Desktop\TR tax system\TR_tax_system-master_201004_ideal\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFABFB62-2567-4CA8-BCFD-76A1364FFBC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774A62A2-9D4D-4A75-A07D-F08854181E43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A28CCFF-135B-4345-98CD-4416B433170E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5A28CCFF-135B-4345-98CD-4416B433170E}"/>
   </bookViews>
   <sheets>
     <sheet name="binek_arac" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -119,7 +117,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -417,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CCE55F-1B0A-4E57-81A5-BBA6925D903A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -462,7 +460,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A069E5F-A95C-4EFD-A754-6B82568E03B6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>